<commit_message>
Fix cardinalité 1..1 (#434)
HealthcareService.providedBy HealthcareService.name & Organization.contact.extension:ror-contact-confidentiality-level e50be969d18206b7a54678b5a6a00f5ce90d4c2d
</commit_message>
<xml_diff>
--- a/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-02T13:26:27+00:00</t>
+    <t>2025-10-02T13:32:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>85</v>
@@ -6474,7 +6474,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>85</v>

</xml_diff>

<commit_message>
change short description of familleActiviteOperationnelle 328bbb4c942d18accfe5c53ab37c2c4369898394
</commit_message>
<xml_diff>
--- a/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-02T13:32:16+00:00</t>
+    <t>2025-10-02T14:00:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -947,7 +947,7 @@
     <t>operationalActivityFamily</t>
   </si>
   <si>
-    <t>familleActiviteOperationnelle (ActiviteOperationnelle) : regroupement cohérent d’activités délivrées dans le cadre d'une prestation, répondant à un besoin de la personne</t>
+    <t>familleActiviteOperationnelle (ActiviteOperationnelle) : Uniquement dans le secteur médico-social, une autre catégorisation des activités peut être renseignée en plus de l'activiteOperationnelle</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J51-FamilleActiviteOperationnelle-ROR/FHIR/JDV-J51-FamilleActiviteOperationnelle-ROR</t>

</xml_diff>

<commit_message>
Fix : typo + cardinalité 0..1 HealthcareService.notAvailable (#436) 122c6db869a20f0152a83c2552ebd94c12cc6849
</commit_message>
<xml_diff>
--- a/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sg/ressources-changes-v43/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-02T14:00:56+00:00</t>
+    <t>2025-10-02T14:19:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -20239,7 +20239,7 @@
         <v>76</v>
       </c>
       <c r="G160" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H160" t="s" s="2">
         <v>86</v>

</xml_diff>